<commit_message>
Burn Down Chart Actualizado
</commit_message>
<xml_diff>
--- a/Burn Down Chart.xlsx
+++ b/Burn Down Chart.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DeoZ1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseluis\Documents\GitHub\Desarrollo_SIS-QSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286ADD5B-A4C0-44A1-9522-75F234EDD6DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B167474-7CCB-4B5C-A75B-0AB4BC67BD94}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -72,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -143,7 +142,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -160,7 +159,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -204,6 +203,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -312,7 +312,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-84F0-45D0-A224-CF021ADBF4DC}"/>
             </c:ext>
@@ -366,11 +366,26 @@
                 <c:pt idx="8">
                   <c:v>55</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-84F0-45D0-A224-CF021ADBF4DC}"/>
             </c:ext>
@@ -385,11 +400,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="477910928"/>
-        <c:axId val="477908632"/>
+        <c:axId val="316650328"/>
+        <c:axId val="316656208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="477910928"/>
+        <c:axId val="316650328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -431,7 +446,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477908632"/>
+        <c:crossAx val="316656208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -439,7 +454,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="477908632"/>
+        <c:axId val="316656208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -490,7 +505,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477910928"/>
+        <c:crossAx val="316650328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -504,6 +519,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -535,14 +551,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1153,7 +1169,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFC07E92-BCD2-4743-B34B-34D6E30718D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BFC07E92-BCD2-4743-B34B-34D6E30718D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1470,11 +1486,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B94062-D1B8-4304-97BC-E6D43AC7F869}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1699,7 +1715,7 @@
         <v>36.3125</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
+        <f>C10-D11</f>
         <v>55</v>
       </c>
       <c r="D11">
@@ -1718,6 +1734,13 @@
         <f t="shared" si="0"/>
         <v>31.125</v>
       </c>
+      <c r="C12">
+        <f t="shared" ref="C12:C16" si="2">C11-D12</f>
+        <v>55</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1727,6 +1750,13 @@
         <f t="shared" si="0"/>
         <v>25.9375</v>
       </c>
+      <c r="C13">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -1736,6 +1766,13 @@
         <f t="shared" si="0"/>
         <v>20.75</v>
       </c>
+      <c r="C14">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -1745,6 +1782,13 @@
         <f t="shared" si="0"/>
         <v>15.5625</v>
       </c>
+      <c r="C15">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -1753,6 +1797,13 @@
       <c r="B16">
         <f t="shared" si="0"/>
         <v>10.375</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>